<commit_message>
Agregada tabla independiente para referentes
</commit_message>
<xml_diff>
--- a/data/bga-metadatos.xlsx
+++ b/data/bga-metadatos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maestría_Lorena\Documents\GitHub\bga-cat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974EDBBF-2368-4F6A-A378-ADD4C008313F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883B82AD-AF63-486B-A3E7-F7E7CED69040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="obras" sheetId="1" r:id="rId1"/>
+    <sheet name="referentes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Título</t>
   </si>
@@ -54,18 +55,12 @@
     <t xml:space="preserve"> suicidas-sisga-1.jpg</t>
   </si>
   <si>
-    <t>Título Referente</t>
-  </si>
-  <si>
     <t>Periódico</t>
   </si>
   <si>
     <t>Doble suicidio en "El Sisga"</t>
   </si>
   <si>
-    <t>Fecha referente</t>
-  </si>
-  <si>
     <t>Junio 29 1965</t>
   </si>
   <si>
@@ -84,21 +79,18 @@
     <t>el-paraiso.jpg</t>
   </si>
   <si>
+    <t>Una indígena y su hijo murieron en persecución</t>
+  </si>
+  <si>
     <t>Mayo 24 del 96</t>
   </si>
   <si>
-    <t>Archivo refetente</t>
+    <t>indigena-hijo-el-tiempo.jpg</t>
   </si>
   <si>
     <t>doble-suicidio-el-tiempo.jpg</t>
   </si>
   <si>
-    <t>Una indígena y su hijo murieron en persecución, Láminas de paisajes latinoamericanos</t>
-  </si>
-  <si>
-    <t>indigena-hijo-el-tiempo.jpg, laminas-paisajes.jpg</t>
-  </si>
-  <si>
     <t>Zócalo de la tragedia</t>
   </si>
   <si>
@@ -115,14 +107,28 @@
   </si>
   <si>
     <t>exmilitar-mata-esposa.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Láminas de paisajes latinoamericanos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> laminas-paisajes.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,8 +156,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAF1907-EE07-4D82-ADB9-AFEA5CC7EE28}">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,33 +492,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>20</v>
-      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -529,72 +528,122 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>1997</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>1983</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B052D09-0F5C-4365-86D8-EC5F5525759B}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
agregados ID y creadas relaciones en la tabla
</commit_message>
<xml_diff>
--- a/data/bga-metadatos.xlsx
+++ b/data/bga-metadatos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maestría_Lorena\Documents\GitHub\bga-cat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883B82AD-AF63-486B-A3E7-F7E7CED69040}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024EA4BE-8130-4DF2-A7B6-56C1BBE0C10B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
   </bookViews>
   <sheets>
     <sheet name="obras" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Título</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t xml:space="preserve"> laminas-paisajes.jpg</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Referentes</t>
   </si>
 </sst>
 </file>
@@ -473,94 +479,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAF1907-EE07-4D82-ADB9-AFEA5CC7EE28}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="55.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>1965</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1997</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G3">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>1983</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -570,75 +599,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B052D09-0F5C-4365-86D8-EC5F5525759B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implementación parcial de Dublin Core
</commit_message>
<xml_diff>
--- a/data/bga-metadatos.xlsx
+++ b/data/bga-metadatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maestría_Lorena\Documents\GitHub\bga-cat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024EA4BE-8130-4DF2-A7B6-56C1BBE0C10B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89744C1C-31DF-48C0-8CDE-565A56A28449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
   </bookViews>
@@ -26,19 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
-  <si>
-    <t>Título</t>
-  </si>
-  <si>
-    <t>Fecha</t>
-  </si>
-  <si>
-    <t>Dimensiones</t>
-  </si>
-  <si>
-    <t>Técnica</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Archivo</t>
   </si>
@@ -46,33 +34,21 @@
     <t>Los Suicidas del Sisga No 1</t>
   </si>
   <si>
-    <t>120x100cm</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Óleo sobre lienzo</t>
   </si>
   <si>
     <t xml:space="preserve"> suicidas-sisga-1.jpg</t>
   </si>
   <si>
-    <t>Periódico</t>
-  </si>
-  <si>
     <t>Doble suicidio en "El Sisga"</t>
   </si>
   <si>
-    <t>Junio 29 1965</t>
-  </si>
-  <si>
     <t>El Tiempo</t>
   </si>
   <si>
     <t xml:space="preserve"> El Paraíso</t>
   </si>
   <si>
-    <t>160x45 cm</t>
-  </si>
-  <si>
     <t>Óleo sobre lienzo</t>
   </si>
   <si>
@@ -82,9 +58,6 @@
     <t>Una indígena y su hijo murieron en persecución</t>
   </si>
   <si>
-    <t>Mayo 24 del 96</t>
-  </si>
-  <si>
     <t>indigena-hijo-el-tiempo.jpg</t>
   </si>
   <si>
@@ -94,9 +67,6 @@
     <t>Zócalo de la tragedia</t>
   </si>
   <si>
-    <t>100x70</t>
-  </si>
-  <si>
     <t>Tipografía sobre papel</t>
   </si>
   <si>
@@ -119,6 +89,30 @@
   </si>
   <si>
     <t>Referentes</t>
+  </si>
+  <si>
+    <t>Ancho cm</t>
+  </si>
+  <si>
+    <t>Alto cm</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creator </t>
+  </si>
+  <si>
+    <t>Beatriz González</t>
+  </si>
+  <si>
+    <t>Format.medium</t>
   </si>
 </sst>
 </file>
@@ -162,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,116 +474,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAF1907-EE07-4D82-ADB9-AFEA5CC7EE28}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>1965</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
+      <c r="E2">
+        <v>120</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
         <v>1997</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3">
+      <c r="E3">
+        <v>160</v>
+      </c>
+      <c r="F3">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
         <v>1983</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4">
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4">
         <v>4</v>
       </c>
     </row>
@@ -615,19 +635,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -635,16 +655,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>23922</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,16 +672,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>35209</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,10 +689,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -680,10 +700,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adición de carpeta web
Se hicieron ajustes en el marco del taller, creando la carpeta web
</commit_message>
<xml_diff>
--- a/data/bga-metadatos.xlsx
+++ b/data/bga-metadatos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maestría_Lorena\Documents\GitHub\bga-cat\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\bga-cat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89744C1C-31DF-48C0-8CDE-565A56A28449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AD7A9D-7A93-48FB-B861-C5E1EEB54A1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A037967C-5925-4B81-9A89-F87F207FD50B}"/>
   </bookViews>
   <sheets>
     <sheet name="obras" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Archivo</t>
   </si>
@@ -82,9 +82,6 @@
     <t xml:space="preserve"> Láminas de paisajes latinoamericanos</t>
   </si>
   <si>
-    <t xml:space="preserve"> laminas-paisajes.jpg</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -113,13 +110,19 @@
   </si>
   <si>
     <t>Format.medium</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>laminas-paisajes.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +132,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,10 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CAF1907-EE07-4D82-ADB9-AFEA5CC7EE28}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,39 +501,41 @@
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.28515625" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="47" customWidth="1"/>
     <col min="12" max="12" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
@@ -530,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -552,6 +566,10 @@
       </c>
       <c r="I2">
         <v>1</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE("https://badac.uniandes.edu.co/files/bga-cat/",E2)</f>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/120</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -559,7 +577,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -581,6 +599,10 @@
       </c>
       <c r="I3">
         <v>2.2999999999999998</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J4" si="0">CONCATENATE("https://badac.uniandes.edu.co/files/bga-cat/",E3)</f>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/160</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -588,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -611,6 +633,13 @@
       <c r="I4">
         <v>4</v>
       </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -619,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B052D09-0F5C-4365-86D8-EC5F5525759B}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,26 +660,30 @@
     <col min="3" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" customWidth="1"/>
     <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="69.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -666,8 +699,12 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>CONCATENATE("https://badac.uniandes.edu.co/files/bga-cat/",E2)</f>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/doble-suicidio-el-tiempo.jpg</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -683,8 +720,12 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F5" si="0">CONCATENATE("https://badac.uniandes.edu.co/files/bga-cat/",E3)</f>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/indigena-hijo-el-tiempo.jpg</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -692,10 +733,14 @@
         <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/laminas-paisajes.jpg</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -705,6 +750,13 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://badac.uniandes.edu.co/files/bga-cat/exmilitar-mata-esposa.jpg</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>